<commit_message>
Set values for EoCSoEVMS and BRAaCTSC to 0
</commit_message>
<xml_diff>
--- a/InputData/trans/EoCSoEVMS/Effect of Charging Stations on EV Market Share.xlsx
+++ b/InputData/trans/EoCSoEVMS/Effect of Charging Stations on EV Market Share.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24131"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox (Energy Innovation)\EI-PlcyMdl\eps-1.5.0-us-wipA\InputData\trans\EoCSoEVMS\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mmahajan\Documents\eps-us\InputData\trans\EoCSoEVMS\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{66484057-564D-40F2-A22E-B23A9D4272A8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25815" windowHeight="11670"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="1" r:id="rId1"/>
@@ -25,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="11">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
   <si>
     <t>EoCSoEVMS Effect of Charging Stations on EV Market Share</t>
   </si>
@@ -33,19 +34,6 @@
     <t>Source:</t>
   </si>
   <si>
-    <t>Page 190, column 2</t>
-  </si>
-  <si>
-    <t>The influence of financial incentives and other socio-economic factors
-on electric vehicle adoption</t>
-  </si>
-  <si>
-    <t>Sierzchula, William; Bakker, Sjoerd; Maat, Kees; Wee, Bert van</t>
-  </si>
-  <si>
-    <t>https://www.sciencedirect.com/science/article/pii/S0301421514000822</t>
-  </si>
-  <si>
     <t>Notes</t>
   </si>
   <si>
@@ -59,13 +47,19 @@
   </si>
   <si>
     <t>1 more charger per 100k pop</t>
+  </si>
+  <si>
+    <t>In the US, we set this to 0 so that increasing EV chargers does not induce additional deployment.</t>
+  </si>
+  <si>
+    <t>None</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="3" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -77,14 +71,6 @@
       <b/>
       <sz val="11"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="11"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -107,26 +93,20 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -404,99 +384,85 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B11"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:XFD7"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="9.140625" style="2"/>
+    <col min="2" max="2" width="9.1796875" style="2"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="2" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A5" s="1" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B4" s="3">
-        <v>2014</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B5" s="2" t="s">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B6" s="4" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B7" s="2" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A9" s="1" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A10" t="s">
+    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A11" t="s">
-        <v>8</v>
-      </c>
-    </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="B6" r:id="rId1"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId2"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <sheetPr>
     <tabColor theme="8" tint="-0.249977111117893"/>
   </sheetPr>
   <dimension ref="A1:B2"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
+    </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="28.28515625" customWidth="1"/>
-    <col min="2" max="2" width="23.140625" customWidth="1"/>
+    <col min="1" max="1" width="28.26953125" customWidth="1"/>
+    <col min="2" max="2" width="23.1796875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="B1" s="7" t="s">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A2" s="6" t="s">
-        <v>10</v>
-      </c>
-      <c r="B2" s="5">
-        <v>1.1999999999999999E-3</v>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="B1" s="5" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
+      <c r="A2" s="4" t="s">
+        <v>6</v>
+      </c>
+      <c r="B2" s="3">
+        <v>0</v>
       </c>
     </row>
   </sheetData>

</xml_diff>